<commit_message>
few new logic and tech fixes 4 sept office
</commit_message>
<xml_diff>
--- a/LOGS/099df001-e23d-427e-8177-ca17d963ab03/main_page_service_output/main_pages.xlsx
+++ b/LOGS/099df001-e23d-427e-8177-ca17d963ab03/main_page_service_output/main_pages.xlsx
@@ -694,7 +694,7 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -711,7 +711,7 @@
         <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -728,7 +728,7 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -745,7 +745,7 @@
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -776,10 +776,10 @@
         <v>615563</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -915,7 +915,7 @@
         <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -932,7 +932,7 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -949,7 +949,7 @@
         <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -983,7 +983,7 @@
         <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1000,7 +1000,7 @@
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:5">

</xml_diff>